<commit_message>
Got the js functions working for the job revenue and expense section.
</commit_message>
<xml_diff>
--- a/Schedule-of-Values-Calculator.xlsx
+++ b/Schedule-of-Values-Calculator.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/stephenlyssy/Software_Projects/ADT_Commercial/Schedule-of-Values-Calculator/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/stephenlyssy/Software_Projects/ADT_Commercial/ADT-SOV-Calculator/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{DEEB7B70-7CE2-DD44-AA42-1A339003104E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DF910E2-9F63-EC42-8447-4ADE838F236E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="500" windowWidth="39980" windowHeight="17380" xr2:uid="{488F5521-3A28-4FFB-8B02-ECE6FA1DD129}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="51200" windowHeight="28800" xr2:uid="{488F5521-3A28-4FFB-8B02-ECE6FA1DD129}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -385,7 +385,7 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
@@ -440,6 +440,7 @@
     <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -759,8 +760,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5ECF7FC2-2601-45F4-976B-4F5C2F259E6F}">
   <dimension ref="A1:G30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -768,7 +769,7 @@
     <col min="1" max="1" width="45.33203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="31.5" customWidth="1"/>
     <col min="4" max="4" width="28" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.1640625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="0" hidden="1" customWidth="1"/>
     <col min="7" max="7" width="10.83203125" hidden="1" customWidth="1"/>
     <col min="8" max="8" width="0" hidden="1" customWidth="1"/>
@@ -828,7 +829,10 @@
       <c r="D5" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="E5" s="12"/>
+      <c r="E5" s="46">
+        <f>SUM(E6:E9)</f>
+        <v>21360</v>
+      </c>
     </row>
     <row r="6" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" s="13" t="s">
@@ -911,7 +915,7 @@
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="E12" s="41">
         <f>SUM(E3:E11)+2400</f>
-        <v>83298.84</v>
+        <v>104658.84</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">
@@ -1068,6 +1072,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100E8298F30E82FEC4FBAB9EEE760829181" ma:contentTypeVersion="13" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="620c88cbbb82f28cef9060856e721204">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="942d8053-4a93-46fc-8ca5-652907ce2e74" xmlns:ns3="a37bc2b5-5908-45eb-bfa1-b82929122f51" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="3eaafbc2c4ddc6500e667a75a639c590" ns2:_="" ns3:_="">
     <xsd:import namespace="942d8053-4a93-46fc-8ca5-652907ce2e74"/>
@@ -1290,22 +1309,24 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{864F7877-4FE4-494C-914D-60B31A4565FB}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2A03B9DF-9FC6-4D5F-826E-C51186B56338}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1C5CDC81-45CC-4777-9B00-72C19A186ACA}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1322,21 +1343,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2A03B9DF-9FC6-4D5F-826E-C51186B56338}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{864F7877-4FE4-494C-914D-60B31A4565FB}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>